<commit_message>
Two new product names added for CCI Sea Ice Conc v1.1 datasets.
</commit_message>
<xml_diff>
--- a/data/cci/cci-product.xlsx
+++ b/data/cci/cci-product.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony.wilson/git/cci-vocabularies2/data/cci/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/diane_knappett_stfc_ac_uk/Documents/Documents/projects/2022_CCI_Open_Data_Portal/vocab_updates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0ECA83B-F5D8-7646-99AD-7B7894EABA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{A0ECA83B-F5D8-7646-99AD-7B7894EABA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A5850F9-71C3-430D-A3A4-C42433DED742}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{04DF87AA-227F-E848-BF0E-6E7C9BB1D368}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{04DF87AA-227F-E848-BF0E-6E7C9BB1D368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="474">
   <si>
     <t>URI</t>
   </si>
@@ -1430,6 +1430,18 @@
   </si>
   <si>
     <t>AVHRR_TIROSN</t>
+  </si>
+  <si>
+    <t>NIMBUS5_ESMR_EASE2_LDTPcorrected_NH</t>
+  </si>
+  <si>
+    <t>NIMBUS5_ESMR_EASE2_LDTPcorrected_SH</t>
+  </si>
+  <si>
+    <t>prod_nimEsmrLCorNH</t>
+  </si>
+  <si>
+    <t>prod_nimEsmrLCorSH</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1670,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1666,13 +1678,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1682,13 +1691,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Accent" xfId="7" xr:uid="{2512F336-722D-FE46-9313-E88B0FECBCED}"/>
@@ -2058,22 +2060,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A059DA7-785A-874C-8D00-32DC40CC12B7}">
-  <dimension ref="A1:AMJ193"/>
+  <dimension ref="A1:AMC195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="A196" sqref="A196"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="50.5" style="2" customWidth="1"/>
-    <col min="5" max="1016" width="10.6640625" style="2" customWidth="1"/>
-    <col min="1017" max="1017" width="13.33203125" style="2" customWidth="1"/>
-    <col min="1018" max="1018" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" style="2" customWidth="1"/>
+    <col min="5" max="1016" width="10.7109375" style="2" customWidth="1"/>
+    <col min="1017" max="1017" width="13.28515625" style="2" customWidth="1"/>
+    <col min="1018" max="1018" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2090,277 +2094,277 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:64" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
@@ -2370,223 +2374,164 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="9"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
-      <c r="AJ26" s="9"/>
-      <c r="AK26" s="9"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
-      <c r="AP26" s="9"/>
-      <c r="AQ26" s="9"/>
-      <c r="AR26" s="9"/>
-      <c r="AS26" s="9"/>
-      <c r="AT26" s="9"/>
-      <c r="AU26" s="9"/>
-      <c r="AV26" s="9"/>
-      <c r="AW26" s="9"/>
-      <c r="AX26" s="9"/>
-      <c r="AY26" s="9"/>
-      <c r="AZ26" s="9"/>
-      <c r="BA26" s="9"/>
-      <c r="BB26" s="9"/>
-      <c r="BC26" s="9"/>
-      <c r="BD26" s="9"/>
-      <c r="BE26" s="9"/>
-      <c r="BF26" s="9"/>
-      <c r="BG26" s="9"/>
-      <c r="BH26" s="9"/>
-      <c r="BI26" s="9"/>
-      <c r="BJ26" s="9"/>
-      <c r="BK26" s="9"/>
-      <c r="BL26" s="9"/>
-    </row>
-    <row r="27" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
+      <c r="AN26" s="2"/>
+      <c r="AO26" s="2"/>
+      <c r="AP26" s="2"/>
+      <c r="AQ26" s="2"/>
+      <c r="AR26" s="2"/>
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="2"/>
+      <c r="BE26" s="2"/>
+      <c r="BF26" s="2"/>
+      <c r="BG26" s="2"/>
+      <c r="BH26" s="2"/>
+      <c r="BI26" s="2"/>
+      <c r="BJ26" s="2"/>
+      <c r="BK26" s="2"/>
+      <c r="BL26" s="2"/>
+    </row>
+    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
-      <c r="AA35" s="9"/>
-      <c r="AB35" s="9"/>
-      <c r="AC35" s="9"/>
-      <c r="AD35" s="9"/>
-      <c r="AE35" s="9"/>
-      <c r="AF35" s="9"/>
-      <c r="AG35" s="9"/>
-      <c r="AH35" s="9"/>
-      <c r="AI35" s="9"/>
-      <c r="AJ35" s="9"/>
-      <c r="AK35" s="9"/>
-      <c r="AL35" s="9"/>
-      <c r="AM35" s="9"/>
-      <c r="AN35" s="9"/>
-      <c r="AO35" s="9"/>
-      <c r="AP35" s="9"/>
-      <c r="AQ35" s="9"/>
-      <c r="AR35" s="9"/>
-      <c r="AS35" s="9"/>
-      <c r="AT35" s="9"/>
-      <c r="AU35" s="9"/>
-      <c r="AV35" s="9"/>
-      <c r="AW35" s="9"/>
-      <c r="AX35" s="9"/>
-      <c r="AY35" s="9"/>
-      <c r="AZ35" s="9"/>
-      <c r="BA35" s="9"/>
-      <c r="BB35" s="9"/>
-      <c r="BC35" s="9"/>
-      <c r="BD35" s="9"/>
-      <c r="BE35" s="9"/>
-      <c r="BF35" s="9"/>
-      <c r="BG35" s="9"/>
-      <c r="BH35" s="9"/>
-      <c r="BI35" s="9"/>
-      <c r="BJ35" s="9"/>
-      <c r="BK35" s="9"/>
-      <c r="BL35" s="9"/>
       <c r="BM35"/>
       <c r="BN35"/>
       <c r="BO35"/>
@@ -3540,83 +3485,17 @@
       <c r="AMA35"/>
       <c r="AMB35"/>
       <c r="AMC35"/>
-      <c r="AMD35" s="11"/>
-      <c r="AME35" s="11"/>
-      <c r="AMF35" s="11"/>
-      <c r="AMG35" s="11"/>
-      <c r="AMH35" s="11"/>
-      <c r="AMI35" s="11"/>
-      <c r="AMJ35" s="11"/>
-    </row>
-    <row r="36" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
-      <c r="AA36" s="9"/>
-      <c r="AB36" s="9"/>
-      <c r="AC36" s="9"/>
-      <c r="AD36" s="9"/>
-      <c r="AE36" s="9"/>
-      <c r="AF36" s="9"/>
-      <c r="AG36" s="9"/>
-      <c r="AH36" s="9"/>
-      <c r="AI36" s="9"/>
-      <c r="AJ36" s="9"/>
-      <c r="AK36" s="9"/>
-      <c r="AL36" s="9"/>
-      <c r="AM36" s="9"/>
-      <c r="AN36" s="9"/>
-      <c r="AO36" s="9"/>
-      <c r="AP36" s="9"/>
-      <c r="AQ36" s="9"/>
-      <c r="AR36" s="9"/>
-      <c r="AS36" s="9"/>
-      <c r="AT36" s="9"/>
-      <c r="AU36" s="9"/>
-      <c r="AV36" s="9"/>
-      <c r="AW36" s="9"/>
-      <c r="AX36" s="9"/>
-      <c r="AY36" s="9"/>
-      <c r="AZ36" s="9"/>
-      <c r="BA36" s="9"/>
-      <c r="BB36" s="9"/>
-      <c r="BC36" s="9"/>
-      <c r="BD36" s="9"/>
-      <c r="BE36" s="9"/>
-      <c r="BF36" s="9"/>
-      <c r="BG36" s="9"/>
-      <c r="BH36" s="9"/>
-      <c r="BI36" s="9"/>
-      <c r="BJ36" s="9"/>
-      <c r="BK36" s="9"/>
-      <c r="BL36" s="9"/>
       <c r="BM36"/>
       <c r="BN36"/>
       <c r="BO36"/>
@@ -4570,83 +4449,17 @@
       <c r="AMA36"/>
       <c r="AMB36"/>
       <c r="AMC36"/>
-      <c r="AMD36" s="11"/>
-      <c r="AME36" s="11"/>
-      <c r="AMF36" s="11"/>
-      <c r="AMG36" s="11"/>
-      <c r="AMH36" s="11"/>
-      <c r="AMI36" s="11"/>
-      <c r="AMJ36" s="11"/>
-    </row>
-    <row r="37" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="6" t="s">
         <v>79</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
-      <c r="Y37" s="9"/>
-      <c r="Z37" s="9"/>
-      <c r="AA37" s="9"/>
-      <c r="AB37" s="9"/>
-      <c r="AC37" s="9"/>
-      <c r="AD37" s="9"/>
-      <c r="AE37" s="9"/>
-      <c r="AF37" s="9"/>
-      <c r="AG37" s="9"/>
-      <c r="AH37" s="9"/>
-      <c r="AI37" s="9"/>
-      <c r="AJ37" s="9"/>
-      <c r="AK37" s="9"/>
-      <c r="AL37" s="9"/>
-      <c r="AM37" s="9"/>
-      <c r="AN37" s="9"/>
-      <c r="AO37" s="9"/>
-      <c r="AP37" s="9"/>
-      <c r="AQ37" s="9"/>
-      <c r="AR37" s="9"/>
-      <c r="AS37" s="9"/>
-      <c r="AT37" s="9"/>
-      <c r="AU37" s="9"/>
-      <c r="AV37" s="9"/>
-      <c r="AW37" s="9"/>
-      <c r="AX37" s="9"/>
-      <c r="AY37" s="9"/>
-      <c r="AZ37" s="9"/>
-      <c r="BA37" s="9"/>
-      <c r="BB37" s="9"/>
-      <c r="BC37" s="9"/>
-      <c r="BD37" s="9"/>
-      <c r="BE37" s="9"/>
-      <c r="BF37" s="9"/>
-      <c r="BG37" s="9"/>
-      <c r="BH37" s="9"/>
-      <c r="BI37" s="9"/>
-      <c r="BJ37" s="9"/>
-      <c r="BK37" s="9"/>
-      <c r="BL37" s="9"/>
       <c r="BM37"/>
       <c r="BN37"/>
       <c r="BO37"/>
@@ -5601,75 +5414,16 @@
       <c r="AMB37"/>
       <c r="AMC37"/>
     </row>
-    <row r="38" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="6" t="s">
         <v>81</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
-      <c r="U38" s="9"/>
-      <c r="V38" s="9"/>
-      <c r="W38" s="9"/>
-      <c r="X38" s="9"/>
-      <c r="Y38" s="9"/>
-      <c r="Z38" s="9"/>
-      <c r="AA38" s="9"/>
-      <c r="AB38" s="9"/>
-      <c r="AC38" s="9"/>
-      <c r="AD38" s="9"/>
-      <c r="AE38" s="9"/>
-      <c r="AF38" s="9"/>
-      <c r="AG38" s="9"/>
-      <c r="AH38" s="9"/>
-      <c r="AI38" s="9"/>
-      <c r="AJ38" s="9"/>
-      <c r="AK38" s="9"/>
-      <c r="AL38" s="9"/>
-      <c r="AM38" s="9"/>
-      <c r="AN38" s="9"/>
-      <c r="AO38" s="9"/>
-      <c r="AP38" s="9"/>
-      <c r="AQ38" s="9"/>
-      <c r="AR38" s="9"/>
-      <c r="AS38" s="9"/>
-      <c r="AT38" s="9"/>
-      <c r="AU38" s="9"/>
-      <c r="AV38" s="9"/>
-      <c r="AW38" s="9"/>
-      <c r="AX38" s="9"/>
-      <c r="AY38" s="9"/>
-      <c r="AZ38" s="9"/>
-      <c r="BA38" s="9"/>
-      <c r="BB38" s="9"/>
-      <c r="BC38" s="9"/>
-      <c r="BD38" s="9"/>
-      <c r="BE38" s="9"/>
-      <c r="BF38" s="9"/>
-      <c r="BG38" s="9"/>
-      <c r="BH38" s="9"/>
-      <c r="BI38" s="9"/>
-      <c r="BJ38" s="9"/>
-      <c r="BK38" s="9"/>
-      <c r="BL38" s="9"/>
       <c r="BM38"/>
       <c r="BN38"/>
       <c r="BO38"/>
@@ -6624,77 +6378,77 @@
       <c r="AMB38"/>
       <c r="AMC38"/>
     </row>
-    <row r="39" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -6707,162 +6461,162 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:1017" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5" t="s">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5" t="s">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5" t="s">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E57" s="5"/>
-    </row>
-    <row r="58" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5" t="s">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:64" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>131</v>
       </c>
@@ -6872,139 +6626,139 @@
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
-      <c r="J59" s="9"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-      <c r="N59" s="9"/>
-      <c r="O59" s="9"/>
-      <c r="P59" s="9"/>
-      <c r="Q59" s="9"/>
-      <c r="R59" s="9"/>
-      <c r="S59" s="9"/>
-      <c r="T59" s="9"/>
-      <c r="U59" s="9"/>
-      <c r="V59" s="9"/>
-      <c r="W59" s="9"/>
-      <c r="X59" s="9"/>
-      <c r="Y59" s="9"/>
-      <c r="Z59" s="9"/>
-      <c r="AA59" s="9"/>
-      <c r="AB59" s="9"/>
-      <c r="AC59" s="9"/>
-      <c r="AD59" s="9"/>
-      <c r="AE59" s="9"/>
-      <c r="AF59" s="9"/>
-      <c r="AG59" s="9"/>
-      <c r="AH59" s="9"/>
-      <c r="AI59" s="9"/>
-      <c r="AJ59" s="9"/>
-      <c r="AK59" s="9"/>
-      <c r="AL59" s="9"/>
-      <c r="AM59" s="9"/>
-      <c r="AN59" s="9"/>
-      <c r="AO59" s="9"/>
-      <c r="AP59" s="9"/>
-      <c r="AQ59" s="9"/>
-      <c r="AR59" s="9"/>
-      <c r="AS59" s="9"/>
-      <c r="AT59" s="9"/>
-      <c r="AU59" s="9"/>
-      <c r="AV59" s="9"/>
-      <c r="AW59" s="9"/>
-      <c r="AX59" s="9"/>
-      <c r="AY59" s="9"/>
-      <c r="AZ59" s="9"/>
-      <c r="BA59" s="9"/>
-      <c r="BB59" s="9"/>
-      <c r="BC59" s="9"/>
-      <c r="BD59" s="9"/>
-      <c r="BE59" s="9"/>
-      <c r="BF59" s="9"/>
-      <c r="BG59" s="9"/>
-      <c r="BH59" s="9"/>
-      <c r="BI59" s="9"/>
-      <c r="BJ59" s="9"/>
-      <c r="BK59" s="9"/>
-      <c r="BL59" s="9"/>
-    </row>
-    <row r="60" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="2"/>
+      <c r="S59" s="2"/>
+      <c r="T59" s="2"/>
+      <c r="U59" s="2"/>
+      <c r="V59" s="2"/>
+      <c r="W59" s="2"/>
+      <c r="X59" s="2"/>
+      <c r="Y59" s="2"/>
+      <c r="Z59" s="2"/>
+      <c r="AA59" s="2"/>
+      <c r="AB59" s="2"/>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="2"/>
+      <c r="AE59" s="2"/>
+      <c r="AF59" s="2"/>
+      <c r="AG59" s="2"/>
+      <c r="AH59" s="2"/>
+      <c r="AI59" s="2"/>
+      <c r="AJ59" s="2"/>
+      <c r="AK59" s="2"/>
+      <c r="AL59" s="2"/>
+      <c r="AM59" s="2"/>
+      <c r="AN59" s="2"/>
+      <c r="AO59" s="2"/>
+      <c r="AP59" s="2"/>
+      <c r="AQ59" s="2"/>
+      <c r="AR59" s="2"/>
+      <c r="AS59" s="2"/>
+      <c r="AT59" s="2"/>
+      <c r="AU59" s="2"/>
+      <c r="AV59" s="2"/>
+      <c r="AW59" s="2"/>
+      <c r="AX59" s="2"/>
+      <c r="AY59" s="2"/>
+      <c r="AZ59" s="2"/>
+      <c r="BA59" s="2"/>
+      <c r="BB59" s="2"/>
+      <c r="BC59" s="2"/>
+      <c r="BD59" s="2"/>
+      <c r="BE59" s="2"/>
+      <c r="BF59" s="2"/>
+      <c r="BG59" s="2"/>
+      <c r="BH59" s="2"/>
+      <c r="BI59" s="2"/>
+      <c r="BJ59" s="2"/>
+      <c r="BK59" s="2"/>
+      <c r="BL59" s="2"/>
+    </row>
+    <row r="60" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-    </row>
-    <row r="62" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="6" t="s">
+      <c r="C63" s="3"/>
+      <c r="D63" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:64" ht="32" x14ac:dyDescent="0.2">
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="8" t="s">
+      <c r="C64" s="3"/>
+      <c r="D64" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:64" ht="32" x14ac:dyDescent="0.2">
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:64" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="8" t="s">
+      <c r="C65" s="3"/>
+      <c r="D65" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -7015,97 +6769,97 @@
       <c r="D66" t="s">
         <v>150</v>
       </c>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-    </row>
-    <row r="68" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-    </row>
-    <row r="69" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-    </row>
-    <row r="71" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-    </row>
-    <row r="72" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-    </row>
-    <row r="73" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-    </row>
-    <row r="74" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-    </row>
-    <row r="75" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>167</v>
       </c>
@@ -7116,20 +6870,20 @@
       <c r="D75" t="s">
         <v>98</v>
       </c>
-      <c r="E75" s="5"/>
-    </row>
-    <row r="76" spans="1:64" ht="15" x14ac:dyDescent="0.2">
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-    </row>
-    <row r="77" spans="1:64" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>171</v>
       </c>
@@ -7139,111 +6893,111 @@
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
-      <c r="N77" s="9"/>
-      <c r="O77" s="9"/>
-      <c r="P77" s="9"/>
-      <c r="Q77" s="9"/>
-      <c r="R77" s="9"/>
-      <c r="S77" s="9"/>
-      <c r="T77" s="9"/>
-      <c r="U77" s="9"/>
-      <c r="V77" s="9"/>
-      <c r="W77" s="9"/>
-      <c r="X77" s="9"/>
-      <c r="Y77" s="9"/>
-      <c r="Z77" s="9"/>
-      <c r="AA77" s="9"/>
-      <c r="AB77" s="9"/>
-      <c r="AC77" s="9"/>
-      <c r="AD77" s="9"/>
-      <c r="AE77" s="9"/>
-      <c r="AF77" s="9"/>
-      <c r="AG77" s="9"/>
-      <c r="AH77" s="9"/>
-      <c r="AI77" s="9"/>
-      <c r="AJ77" s="9"/>
-      <c r="AK77" s="9"/>
-      <c r="AL77" s="9"/>
-      <c r="AM77" s="9"/>
-      <c r="AN77" s="9"/>
-      <c r="AO77" s="9"/>
-      <c r="AP77" s="9"/>
-      <c r="AQ77" s="9"/>
-      <c r="AR77" s="9"/>
-      <c r="AS77" s="9"/>
-      <c r="AT77" s="9"/>
-      <c r="AU77" s="9"/>
-      <c r="AV77" s="9"/>
-      <c r="AW77" s="9"/>
-      <c r="AX77" s="9"/>
-      <c r="AY77" s="9"/>
-      <c r="AZ77" s="9"/>
-      <c r="BA77" s="9"/>
-      <c r="BB77" s="9"/>
-      <c r="BC77" s="9"/>
-      <c r="BD77" s="9"/>
-      <c r="BE77" s="9"/>
-      <c r="BF77" s="9"/>
-      <c r="BG77" s="9"/>
-      <c r="BH77" s="9"/>
-      <c r="BI77" s="9"/>
-      <c r="BJ77" s="9"/>
-      <c r="BK77" s="9"/>
-      <c r="BL77" s="9"/>
-    </row>
-    <row r="78" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="2"/>
+      <c r="S77" s="2"/>
+      <c r="T77" s="2"/>
+      <c r="U77" s="2"/>
+      <c r="V77" s="2"/>
+      <c r="W77" s="2"/>
+      <c r="X77" s="2"/>
+      <c r="Y77" s="2"/>
+      <c r="Z77" s="2"/>
+      <c r="AA77" s="2"/>
+      <c r="AB77" s="2"/>
+      <c r="AC77" s="2"/>
+      <c r="AD77" s="2"/>
+      <c r="AE77" s="2"/>
+      <c r="AF77" s="2"/>
+      <c r="AG77" s="2"/>
+      <c r="AH77" s="2"/>
+      <c r="AI77" s="2"/>
+      <c r="AJ77" s="2"/>
+      <c r="AK77" s="2"/>
+      <c r="AL77" s="2"/>
+      <c r="AM77" s="2"/>
+      <c r="AN77" s="2"/>
+      <c r="AO77" s="2"/>
+      <c r="AP77" s="2"/>
+      <c r="AQ77" s="2"/>
+      <c r="AR77" s="2"/>
+      <c r="AS77" s="2"/>
+      <c r="AT77" s="2"/>
+      <c r="AU77" s="2"/>
+      <c r="AV77" s="2"/>
+      <c r="AW77" s="2"/>
+      <c r="AX77" s="2"/>
+      <c r="AY77" s="2"/>
+      <c r="AZ77" s="2"/>
+      <c r="BA77" s="2"/>
+      <c r="BB77" s="2"/>
+      <c r="BC77" s="2"/>
+      <c r="BD77" s="2"/>
+      <c r="BE77" s="2"/>
+      <c r="BF77" s="2"/>
+      <c r="BG77" s="2"/>
+      <c r="BH77" s="2"/>
+      <c r="BI77" s="2"/>
+      <c r="BJ77" s="2"/>
+      <c r="BK77" s="2"/>
+      <c r="BL77" s="2"/>
+    </row>
+    <row r="78" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B78" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-    </row>
-    <row r="79" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B79" s="7" t="s">
+      <c r="B79" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-    </row>
-    <row r="80" spans="1:64" ht="16" x14ac:dyDescent="0.2">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B80" s="7" t="s">
+      <c r="B80" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-    </row>
-    <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-    </row>
-    <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>181</v>
       </c>
@@ -7254,9 +7008,9 @@
       <c r="D82" t="s">
         <v>183</v>
       </c>
-      <c r="E82" s="5"/>
-    </row>
-    <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>184</v>
       </c>
@@ -7267,127 +7021,127 @@
       <c r="D83" t="s">
         <v>186</v>
       </c>
-      <c r="E83" s="5"/>
-    </row>
-    <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E83" s="3"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-    </row>
-    <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="5"/>
-    </row>
-    <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5" t="s">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="E86" s="5"/>
-    </row>
-    <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5" t="s">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E87" s="5"/>
-    </row>
-    <row r="88" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="6" t="s">
+      <c r="C88" s="3"/>
+      <c r="D88" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="E88" s="5"/>
-    </row>
-    <row r="89" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="6" t="s">
+      <c r="C89" s="3"/>
+      <c r="D89" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="E89" s="5"/>
-    </row>
-    <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-    </row>
-    <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-    </row>
-    <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
-    </row>
-    <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-    </row>
-    <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>211</v>
       </c>
@@ -7398,42 +7152,42 @@
       <c r="D94" t="s">
         <v>213</v>
       </c>
-      <c r="E94" s="5"/>
-    </row>
-    <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="5"/>
-    </row>
-    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-    </row>
-    <row r="97" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C97" s="5"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
-    </row>
-    <row r="98" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>220</v>
       </c>
@@ -7444,123 +7198,123 @@
       <c r="D98" t="s">
         <v>222</v>
       </c>
-      <c r="E98" s="5"/>
-    </row>
-    <row r="99" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E98" s="3"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-    </row>
-    <row r="100" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="B100" s="8" t="s">
+      <c r="B100" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-    </row>
-    <row r="101" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-    </row>
-    <row r="102" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-    </row>
-    <row r="103" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5" t="s">
+      <c r="C103" s="3"/>
+      <c r="D103" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="E103" s="5"/>
-    </row>
-    <row r="104" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E103" s="3"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5" t="s">
+      <c r="C104" s="3"/>
+      <c r="D104" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E104" s="5"/>
-    </row>
-    <row r="105" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E104" s="3"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-    </row>
-    <row r="106" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B106" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-    </row>
-    <row r="107" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B107" s="7" t="s">
+      <c r="B107" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
-      <c r="E107" s="5"/>
-    </row>
-    <row r="108" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
-      <c r="E108" s="5"/>
-    </row>
-    <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>245</v>
       </c>
@@ -7571,10 +7325,10 @@
       <c r="D109" t="s">
         <v>247</v>
       </c>
-      <c r="E109" s="5"/>
-    </row>
-    <row r="110" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A110" s="9" t="s">
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>248</v>
       </c>
       <c r="B110" s="2" t="s">
@@ -7584,7 +7338,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>251</v>
       </c>
@@ -7592,7 +7346,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>253</v>
       </c>
@@ -7603,7 +7357,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>256</v>
       </c>
@@ -7614,7 +7368,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>259</v>
       </c>
@@ -7625,7 +7379,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>262</v>
       </c>
@@ -7636,7 +7390,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>265</v>
       </c>
@@ -7647,7 +7401,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>268</v>
       </c>
@@ -7658,7 +7412,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>271</v>
       </c>
@@ -7669,7 +7423,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>274</v>
       </c>
@@ -7680,7 +7434,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>277</v>
       </c>
@@ -7691,7 +7445,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>280</v>
       </c>
@@ -7699,7 +7453,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>282</v>
       </c>
@@ -7707,7 +7461,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>284</v>
       </c>
@@ -7715,7 +7469,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>286</v>
       </c>
@@ -7723,7 +7477,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>288</v>
       </c>
@@ -7731,7 +7485,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>290</v>
       </c>
@@ -7742,7 +7496,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>293</v>
       </c>
@@ -7750,7 +7504,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>295</v>
       </c>
@@ -7758,7 +7512,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>297</v>
       </c>
@@ -7766,7 +7520,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>299</v>
       </c>
@@ -7774,7 +7528,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>301</v>
       </c>
@@ -7785,7 +7539,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>304</v>
       </c>
@@ -7796,7 +7550,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>307</v>
       </c>
@@ -7807,7 +7561,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>310</v>
       </c>
@@ -7818,7 +7572,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>313</v>
       </c>
@@ -7829,7 +7583,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>316</v>
       </c>
@@ -7840,7 +7594,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>319</v>
       </c>
@@ -7851,7 +7605,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>322</v>
       </c>
@@ -7862,7 +7616,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>325</v>
       </c>
@@ -7873,7 +7627,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>328</v>
       </c>
@@ -7884,7 +7638,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>331</v>
       </c>
@@ -7895,7 +7649,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>334</v>
       </c>
@@ -7906,7 +7660,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>337</v>
       </c>
@@ -7917,7 +7671,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>340</v>
       </c>
@@ -7928,7 +7682,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>343</v>
       </c>
@@ -7939,7 +7693,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>346</v>
       </c>
@@ -7950,7 +7704,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>349</v>
       </c>
@@ -7961,7 +7715,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>352</v>
       </c>
@@ -7972,7 +7726,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>355</v>
       </c>
@@ -7983,7 +7737,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>358</v>
       </c>
@@ -7994,7 +7748,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>361</v>
       </c>
@@ -8005,7 +7759,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>364</v>
       </c>
@@ -8016,7 +7770,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>367</v>
       </c>
@@ -8027,7 +7781,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>370</v>
       </c>
@@ -8038,7 +7792,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>373</v>
       </c>
@@ -8049,7 +7803,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>376</v>
       </c>
@@ -8060,7 +7814,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>379</v>
       </c>
@@ -8071,7 +7825,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>382</v>
       </c>
@@ -8082,7 +7836,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>385</v>
       </c>
@@ -8093,7 +7847,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>388</v>
       </c>
@@ -8104,40 +7858,40 @@
         <v>390</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>391</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="D161" s="8" t="s">
+      <c r="D161" s="7" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>394</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="D162" s="8" t="s">
+      <c r="D162" s="7" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>397</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="D163" s="8" t="s">
+      <c r="D163" s="7" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>400</v>
       </c>
@@ -8148,7 +7902,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>403</v>
       </c>
@@ -8159,7 +7913,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>405</v>
       </c>
@@ -8170,7 +7924,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>407</v>
       </c>
@@ -8178,7 +7932,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>409</v>
       </c>
@@ -8186,7 +7940,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>411</v>
       </c>
@@ -8197,7 +7951,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>414</v>
       </c>
@@ -8208,7 +7962,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>417</v>
       </c>
@@ -8219,7 +7973,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>420</v>
       </c>
@@ -8230,7 +7984,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>423</v>
       </c>
@@ -8241,7 +7995,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>426</v>
       </c>
@@ -8252,7 +8006,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>429</v>
       </c>
@@ -8263,7 +8017,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>432</v>
       </c>
@@ -8274,7 +8028,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>435</v>
       </c>
@@ -8285,7 +8039,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>438</v>
       </c>
@@ -8293,7 +8047,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>440</v>
       </c>
@@ -8301,7 +8055,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>442</v>
       </c>
@@ -8309,7 +8063,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>444</v>
       </c>
@@ -8317,7 +8071,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>446</v>
       </c>
@@ -8325,7 +8079,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>448</v>
       </c>
@@ -8333,7 +8087,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>450</v>
       </c>
@@ -8341,7 +8095,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>452</v>
       </c>
@@ -8349,7 +8103,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>454</v>
       </c>
@@ -8357,7 +8111,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>456</v>
       </c>
@@ -8365,7 +8119,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>458</v>
       </c>
@@ -8373,7 +8127,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>460</v>
       </c>
@@ -8381,7 +8135,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>462</v>
       </c>
@@ -8389,7 +8143,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>464</v>
       </c>
@@ -8397,7 +8151,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>466</v>
       </c>
@@ -8405,12 +8159,28 @@
         <v>467</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>468</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>469</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added product string for snow products
</commit_message>
<xml_diff>
--- a/data/cci/cci-product.xlsx
+++ b/data/cci/cci-product.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/alison_waterfall_stfc_ac_uk/Documents/Documents/GitHub/cci-vocabularies/data/cci/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amw23\AppData\Roaming\MobaXterm\slash\RemoteFiles\264094_5_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{E2C577A2-6DCC-4863-B9A9-FA02136E6212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2CED3B9-5691-489C-A84F-6D9D802D9705}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8698D110-CEA0-44F5-A4A0-4B424D64BB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{04DF87AA-227F-E848-BF0E-6E7C9BB1D368}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{04DF87AA-227F-E848-BF0E-6E7C9BB1D368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="484">
   <si>
     <t>URI</t>
   </si>
@@ -1466,6 +1466,12 @@
   </si>
   <si>
     <t>prod_iasiMopittLatmos1M</t>
+  </si>
+  <si>
+    <t>prod_slstrS3</t>
+  </si>
+  <si>
+    <t>SLSTR_S3</t>
   </si>
 </sst>
 </file>
@@ -2084,10 +2090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A059DA7-785A-874C-8D00-32DC40CC12B7}">
-  <dimension ref="A1:AMC198"/>
+  <dimension ref="A1:AMC199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8237,6 +8243,14 @@
         <v>480</v>
       </c>
     </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="1.143700787401575" bottom="1.143700787401575" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>